<commit_message>
editted data and added note in script
</commit_message>
<xml_diff>
--- a/data/01_pd-samples/25_10-16_pd_samples-edited.xlsx
+++ b/data/01_pd-samples/25_10-16_pd_samples-edited.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caprinapugliese/Documents/School/Uconn/2024-26_Grad_School/Dagilis-lab/WNS-project/data/01_pd-samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D700BA-60D2-714E-8DEE-7D0AFA95AF8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCA3D26-0134-0445-8385-6D6FD08E9F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="37220" windowHeight="21100" xr2:uid="{D99E271A-162C-F24C-8D0E-BBA6ED327C07}"/>
   </bookViews>
@@ -1826,14 +1826,14 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1858,7 +1858,7 @@
     <tableColumn id="1" xr3:uid="{30EFF156-3D30-484A-8AD7-EA85D1CE06B4}" name="sample_id"/>
     <tableColumn id="2" xr3:uid="{A57D6E87-53D9-9040-A419-D8F9EB108C4C}" name="individuals"/>
     <tableColumn id="24" xr3:uid="{3B742AA1-E6CD-E149-8D76-9BF45791B0CA}" name="names"/>
-    <tableColumn id="23" xr3:uid="{696A16A2-3458-2749-BBFE-412CD7189CD5}" name="sra_number" dataDxfId="0"/>
+    <tableColumn id="23" xr3:uid="{696A16A2-3458-2749-BBFE-412CD7189CD5}" name="sra_number" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{2A54557F-8AB7-7F43-877C-FD7C0EA8D35A}" name="sra" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{BDE76617-CD6A-DC47-AB84-5ECFBE4656EA}" name="platform"/>
     <tableColumn id="5" xr3:uid="{8E9655EC-1F75-A54B-A3E9-4D24F04D79E1}" name="library"/>
@@ -1877,7 +1877,7 @@
     <tableColumn id="19" xr3:uid="{180BBF41-7859-AE4D-9DB9-B4899CCD75FC}" name="sra_project"/>
     <tableColumn id="15" xr3:uid="{C8CDD26B-E025-644D-850C-479D08FC207A}" name="provider"/>
     <tableColumn id="21" xr3:uid="{1F073B69-2EEB-4F4E-A4F7-CF5A32E0C613}" name="strain"/>
-    <tableColumn id="16" xr3:uid="{5A8723C2-EA7F-804A-A08F-C0FD996227E9}" name="citation" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{5A8723C2-EA7F-804A-A08F-C0FD996227E9}" name="citation" dataDxfId="0"/>
     <tableColumn id="17" xr3:uid="{804E7016-075C-2E4B-B8E7-6333BEF7B9EA}" name="notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2203,8 +2203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E4D9535-1238-AB48-B467-419735026371}">
   <dimension ref="A1:X75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2635,7 +2635,7 @@
       <c r="B7" t="s">
         <v>132</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="7" t="s">
         <v>131</v>
       </c>
       <c r="D7" s="5">
@@ -2703,7 +2703,7 @@
       <c r="B8" t="s">
         <v>136</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="7" t="s">
         <v>135</v>
       </c>
       <c r="D8" s="5">
@@ -2768,7 +2768,7 @@
       <c r="B9" t="s">
         <v>140</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="7" t="s">
         <v>139</v>
       </c>
       <c r="D9" s="5">
@@ -2833,7 +2833,7 @@
       <c r="B10" t="s">
         <v>144</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="7" t="s">
         <v>143</v>
       </c>
       <c r="D10" s="5">
@@ -2898,7 +2898,7 @@
       <c r="B11" t="s">
         <v>148</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="7" t="s">
         <v>147</v>
       </c>
       <c r="D11" s="5">
@@ -2963,7 +2963,7 @@
       <c r="B12" t="s">
         <v>151</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="7" t="s">
         <v>126</v>
       </c>
       <c r="D12" s="5">
@@ -3028,7 +3028,7 @@
       <c r="B13" t="s">
         <v>127</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="7" t="s">
         <v>126</v>
       </c>
       <c r="D13" s="5">

</xml_diff>